<commit_message>
Se activa la actualización automática de las tablas Fails y Totales al momento de abrir el archivo de excel.
</commit_message>
<xml_diff>
--- a/REPORTE_SQL_CHECADORES.xlsx
+++ b/REPORTE_SQL_CHECADORES.xlsx
@@ -3478,7 +3478,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B8DDB95-6733-483E-8299-B6FB8FAB1DDF}" name="Tabla_Consulta_desde_Biostar" displayName="Tabla_Consulta_desde_Biostar" ref="A6:E1053" tableType="queryTable" totalsRowCount="1">
-  <autoFilter ref="A6:E1052" xr:uid="{B994A696-D6A9-492D-B59D-E5371DE2CB18}"/>
+  <autoFilter ref="A6:E1052" xr:uid="{69C4BF98-4BD8-4E12-9901-CD1F540B9CBA}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DA42567C-6D39-496E-947D-B7E001AD0FA9}" uniqueName="1" name="Date" totalsRowLabel="Total" queryTableFieldId="1" dataDxfId="4" totalsRowDxfId="5"/>
     <tableColumn id="2" xr3:uid="{0149E631-A9FD-4E6C-8AA5-B63A92728941}" uniqueName="2" name="Device" queryTableFieldId="2"/>
@@ -3492,7 +3492,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2F212703-9A35-45BA-AA18-AFCEB663DE06}" name="Tabla_Consulta_desde_Biostar3" displayName="Tabla_Consulta_desde_Biostar3" ref="A6:C40" tableType="queryTable" totalsRowCount="1" totalsRowDxfId="7">
-  <autoFilter ref="A6:C39" xr:uid="{1CD0B457-6774-4ABF-9F58-956995BAF1DE}"/>
+  <autoFilter ref="A6:C39" xr:uid="{79E92496-9672-4B0D-834F-93480B5A88AC}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{4551646C-C5A5-455B-90AC-7CA4DD388180}" uniqueName="1" name="Date" totalsRowLabel="Total" queryTableFieldId="1" dataDxfId="0" totalsRowDxfId="1"/>
     <tableColumn id="2" xr3:uid="{65DCE6A0-4B04-45C8-B253-540A4806C45C}" uniqueName="2" name="Device" queryTableFieldId="2" totalsRowDxfId="2"/>

</xml_diff>